<commit_message>
Added Addmoney + Recharge cases
</commit_message>
<xml_diff>
--- a/AndroidApp/Parameters/TestDataSheet.xlsx
+++ b/AndroidApp/Parameters/TestDataSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="146">
   <si>
     <t xml:space="preserve">Sno</t>
   </si>
@@ -69,13 +69,10 @@
     <t xml:space="preserve">valid login using email</t>
   </si>
   <si>
-    <t xml:space="preserve">7835053234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manoj.amurocker@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smlove_0571</t>
+    <t xml:space="preserve">rush2ash@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuesday20</t>
   </si>
   <si>
     <t xml:space="preserve">8527797582</t>
@@ -195,31 +192,31 @@
     <t xml:space="preserve">5</t>
   </si>
   <si>
-    <t xml:space="preserve">ICICI</t>
+    <t xml:space="preserve">ICICI Bank</t>
   </si>
   <si>
     <t xml:space="preserve">https://shopping.icicibank.com/corp/BANKAWAY</t>
   </si>
   <si>
-    <t xml:space="preserve">HDF</t>
+    <t xml:space="preserve">HDFC Bank</t>
   </si>
   <si>
     <t xml:space="preserve">https://netbanking.hdfcbank.com/netbanking/merchant</t>
   </si>
   <si>
-    <t xml:space="preserve">CITIBK</t>
+    <t xml:space="preserve">CitiBank</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.citibank.co.in/servlets/TransReq</t>
   </si>
   <si>
-    <t xml:space="preserve">AXIS</t>
+    <t xml:space="preserve">Axis Bank</t>
   </si>
   <si>
     <t xml:space="preserve">retail.axisbank.co.in</t>
   </si>
   <si>
-    <t xml:space="preserve">PNB</t>
+    <t xml:space="preserve">Allahabad Bank</t>
   </si>
   <si>
     <t xml:space="preserve">netpnb</t>
@@ -476,7 +473,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -497,6 +494,87 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -520,20 +598,77 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -544,7 +679,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -568,25 +703,73 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -594,11 +777,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,33 +793,49 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="22">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -648,7 +847,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -664,7 +863,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -693,8 +892,8 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -769,14 +968,14 @@
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1" t="n">
+        <v>9953138474</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>11</v>
@@ -796,16 +995,16 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>2</v>
@@ -819,13 +1018,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
@@ -845,13 +1044,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
@@ -874,10 +1073,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
@@ -893,20 +1092,23 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
       <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>2</v>
@@ -917,10 +1119,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" display="mayank.suneja@mobikwik.com"/>
-    <hyperlink ref="D5" r:id="rId2" display="rashia15@gmail.com"/>
-    <hyperlink ref="D8" r:id="rId3" display="par.ajjain@gmail.com"/>
-    <hyperlink ref="E8" r:id="rId4" display="Test@1234"/>
+    <hyperlink ref="D3" r:id="rId1" display="rush2ash@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId2" display="mayank.suneja@mobikwik.com"/>
+    <hyperlink ref="D5" r:id="rId3" display="rashia15@gmail.com"/>
+    <hyperlink ref="D8" r:id="rId4" display="par.ajjain@gmail.com"/>
+    <hyperlink ref="E8" r:id="rId5" display="Test@1234"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -960,22 +1163,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -983,22 +1186,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1006,22 +1209,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1042,8 +1245,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1051,7 +1254,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="42.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="7" style="0" width="8.52"/>
@@ -1064,34 +1267,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,16 +1302,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>11</v>
@@ -1134,16 +1337,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>11</v>
@@ -1169,16 +1372,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>11</v>
@@ -1204,16 +1407,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>11</v>
@@ -1239,16 +1442,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>11</v>
@@ -1274,30 +1477,30 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,30 +1508,30 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1370,69 +1573,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>9</v>
@@ -1473,34 +1676,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,31 +1711,31 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,31 +1743,31 @@
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>103</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1572,31 +1775,31 @@
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I4" s="0" t="s">
+      <c r="J4" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,31 +1807,31 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1636,25 +1839,25 @@
         <v>5</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="I6" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,25 +1865,25 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>133</v>
-      </c>
       <c r="I7" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1688,25 +1891,25 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="E8" s="8" t="s">
+      <c r="F8" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>137</v>
-      </c>
       <c r="H8" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,25 +1917,25 @@
         <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" s="8" t="s">
+      <c r="F9" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>140</v>
-      </c>
       <c r="G9" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H9" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,25 +1943,25 @@
         <v>9</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="F10" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="G10" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>144</v>
-      </c>
       <c r="I10" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1796,24 +1999,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>